<commit_message>
update Ligue1 output files
</commit_message>
<xml_diff>
--- a/FantaSoccer/MyModule/Ligue1/Results_Giornata_18_2020.xlsx
+++ b/FantaSoccer/MyModule/Ligue1/Results_Giornata_18_2020.xlsx
@@ -2252,7 +2252,7 @@
         <v>584</v>
       </c>
       <c r="G3">
-        <v>6.065016152388197</v>
+        <v>6.065016152388195</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2275,7 +2275,7 @@
         <v>584</v>
       </c>
       <c r="G4">
-        <v>5.781763180839364</v>
+        <v>5.781763180839362</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2298,7 +2298,7 @@
         <v>584</v>
       </c>
       <c r="G5">
-        <v>5.941353137555365</v>
+        <v>5.941353137555363</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2321,7 +2321,7 @@
         <v>584</v>
       </c>
       <c r="G6">
-        <v>5.716766266134782</v>
+        <v>5.716766266134781</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2344,7 +2344,7 @@
         <v>584</v>
       </c>
       <c r="G7">
-        <v>5.895980716410116</v>
+        <v>5.895980716410114</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2390,7 +2390,7 @@
         <v>584</v>
       </c>
       <c r="G9">
-        <v>5.785156213730095</v>
+        <v>5.785156213730093</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2413,7 +2413,7 @@
         <v>584</v>
       </c>
       <c r="G10">
-        <v>5.934640439924611</v>
+        <v>5.93464043992461</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2459,7 +2459,7 @@
         <v>584</v>
       </c>
       <c r="G12">
-        <v>5.847104555413844</v>
+        <v>5.847104555413842</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2482,7 +2482,7 @@
         <v>584</v>
       </c>
       <c r="G13">
-        <v>5.88821072965687</v>
+        <v>5.888210729656868</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2574,7 +2574,7 @@
         <v>584</v>
       </c>
       <c r="G17">
-        <v>5.895980716410116</v>
+        <v>5.895980716410114</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2666,7 +2666,7 @@
         <v>584</v>
       </c>
       <c r="G21">
-        <v>5.505060447916567</v>
+        <v>5.505060447916565</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2735,7 +2735,7 @@
         <v>584</v>
       </c>
       <c r="G24">
-        <v>5.895980716410116</v>
+        <v>5.895980716410114</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2804,7 +2804,7 @@
         <v>584</v>
       </c>
       <c r="G27">
-        <v>5.895980716410116</v>
+        <v>5.895980716410114</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2827,7 +2827,7 @@
         <v>584</v>
       </c>
       <c r="G28">
-        <v>5.513587746994953</v>
+        <v>5.513587746994951</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2850,7 +2850,7 @@
         <v>584</v>
       </c>
       <c r="G29">
-        <v>5.800136991892283</v>
+        <v>5.800136991892281</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2873,7 +2873,7 @@
         <v>584</v>
       </c>
       <c r="G30">
-        <v>5.895980716410116</v>
+        <v>5.895980716410114</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2896,7 +2896,7 @@
         <v>584</v>
       </c>
       <c r="G31">
-        <v>5.835249915389228</v>
+        <v>5.835249915389226</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2916,7 +2916,7 @@
         <v>585</v>
       </c>
       <c r="G32">
-        <v>5.904885639645305</v>
+        <v>5.904885639645303</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2939,7 +2939,7 @@
         <v>585</v>
       </c>
       <c r="G33">
-        <v>6.01670376326786</v>
+        <v>6.016703763267858</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2985,7 +2985,7 @@
         <v>585</v>
       </c>
       <c r="G35">
-        <v>6.2885745702289</v>
+        <v>6.288574570228902</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3008,7 +3008,7 @@
         <v>585</v>
       </c>
       <c r="G36">
-        <v>5.937307824478418</v>
+        <v>5.937307824478416</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3054,7 +3054,7 @@
         <v>585</v>
       </c>
       <c r="G38">
-        <v>5.826978382467158</v>
+        <v>5.826978382467156</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3189,7 +3189,7 @@
         <v>585</v>
       </c>
       <c r="G44">
-        <v>5.771511622732956</v>
+        <v>5.771511622732954</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3255,7 +3255,7 @@
         <v>585</v>
       </c>
       <c r="G47">
-        <v>6.38240209491006</v>
+        <v>6.382402094910058</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3278,7 +3278,7 @@
         <v>585</v>
       </c>
       <c r="G48">
-        <v>6.020444401703942</v>
+        <v>6.02044440170394</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3321,7 +3321,7 @@
         <v>585</v>
       </c>
       <c r="G50">
-        <v>6.069878472350596</v>
+        <v>6.069878472350594</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3367,7 +3367,7 @@
         <v>585</v>
       </c>
       <c r="G52">
-        <v>5.971800281607647</v>
+        <v>5.971800281607645</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -3479,7 +3479,7 @@
         <v>586</v>
       </c>
       <c r="G57">
-        <v>5.956885886081509</v>
+        <v>5.956885886081504</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -3502,7 +3502,7 @@
         <v>586</v>
       </c>
       <c r="G58">
-        <v>5.605657714913796</v>
+        <v>5.605657714913792</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3525,7 +3525,7 @@
         <v>586</v>
       </c>
       <c r="G59">
-        <v>6.066501045719204</v>
+        <v>6.066501045719202</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3548,7 +3548,7 @@
         <v>586</v>
       </c>
       <c r="G60">
-        <v>6.011301524866083</v>
+        <v>6.01130152486608</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3571,7 +3571,7 @@
         <v>586</v>
       </c>
       <c r="G61">
-        <v>5.922600107735806</v>
+        <v>5.922600107735801</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3594,7 +3594,7 @@
         <v>586</v>
       </c>
       <c r="G62">
-        <v>5.968875157234078</v>
+        <v>5.968875157234073</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3617,7 +3617,7 @@
         <v>586</v>
       </c>
       <c r="G63">
-        <v>6.136161554577584</v>
+        <v>6.136161554577581</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3640,7 +3640,7 @@
         <v>586</v>
       </c>
       <c r="G64">
-        <v>5.672699082199075</v>
+        <v>5.672699082199069</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3663,7 +3663,7 @@
         <v>586</v>
       </c>
       <c r="G65">
-        <v>6.136274676577977</v>
+        <v>6.136274676577972</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3686,7 +3686,7 @@
         <v>586</v>
       </c>
       <c r="G66">
-        <v>5.599361842805849</v>
+        <v>5.599361842805844</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3709,7 +3709,7 @@
         <v>586</v>
       </c>
       <c r="G67">
-        <v>6.272449562701731</v>
+        <v>6.27244956270173</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3732,7 +3732,7 @@
         <v>586</v>
       </c>
       <c r="G68">
-        <v>6.027704396195566</v>
+        <v>6.027704396195561</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3755,7 +3755,7 @@
         <v>586</v>
       </c>
       <c r="G69">
-        <v>6.222750264890496</v>
+        <v>6.22275026489049</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3778,7 +3778,7 @@
         <v>586</v>
       </c>
       <c r="G70">
-        <v>5.879193361575058</v>
+        <v>5.879193361575052</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3801,7 +3801,7 @@
         <v>586</v>
       </c>
       <c r="G71">
-        <v>5.937043324574424</v>
+        <v>5.937043324574421</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3824,7 +3824,7 @@
         <v>586</v>
       </c>
       <c r="G72">
-        <v>5.892170793603902</v>
+        <v>5.892170793603898</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3847,7 +3847,7 @@
         <v>586</v>
       </c>
       <c r="G73">
-        <v>5.918607152658828</v>
+        <v>5.918607152658821</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3870,7 +3870,7 @@
         <v>586</v>
       </c>
       <c r="G74">
-        <v>5.85085300112415</v>
+        <v>5.850853001124146</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3893,7 +3893,7 @@
         <v>586</v>
       </c>
       <c r="G75">
-        <v>6.087111576498745</v>
+        <v>6.087111576498741</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3916,7 +3916,7 @@
         <v>586</v>
       </c>
       <c r="G76">
-        <v>5.879193361575058</v>
+        <v>5.879193361575052</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3939,7 +3939,7 @@
         <v>586</v>
       </c>
       <c r="G77">
-        <v>6.437706642451341</v>
+        <v>6.437706642451338</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3959,7 +3959,7 @@
         <v>586</v>
       </c>
       <c r="G78">
-        <v>5.892170793603902</v>
+        <v>5.892170793603898</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3982,7 +3982,7 @@
         <v>586</v>
       </c>
       <c r="G79">
-        <v>5.94758330917037</v>
+        <v>5.947583309170365</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -4005,7 +4005,7 @@
         <v>586</v>
       </c>
       <c r="G80">
-        <v>5.892170793603902</v>
+        <v>5.892170793603898</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -4028,7 +4028,7 @@
         <v>586</v>
       </c>
       <c r="G81">
-        <v>5.892170793603902</v>
+        <v>5.892170793603898</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4051,7 +4051,7 @@
         <v>586</v>
       </c>
       <c r="G82">
-        <v>5.889525787904883</v>
+        <v>5.889525787904879</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4074,7 +4074,7 @@
         <v>586</v>
       </c>
       <c r="G83">
-        <v>5.876423363732358</v>
+        <v>5.876423363732353</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -4097,7 +4097,7 @@
         <v>586</v>
       </c>
       <c r="G84">
-        <v>5.892170793603902</v>
+        <v>5.892170793603898</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4120,7 +4120,7 @@
         <v>587</v>
       </c>
       <c r="G85">
-        <v>5.988229988663314</v>
+        <v>5.988229988663316</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4143,7 +4143,7 @@
         <v>587</v>
       </c>
       <c r="G86">
-        <v>6.051177315072557</v>
+        <v>6.05117731507256</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4166,7 +4166,7 @@
         <v>587</v>
       </c>
       <c r="G87">
-        <v>5.854242457526129</v>
+        <v>5.854242457526133</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4189,7 +4189,7 @@
         <v>587</v>
       </c>
       <c r="G88">
-        <v>5.960630424603752</v>
+        <v>5.96063042460375</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -4212,7 +4212,7 @@
         <v>588</v>
       </c>
       <c r="G89">
-        <v>5.960630424603752</v>
+        <v>5.96063042460375</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -4235,7 +4235,7 @@
         <v>587</v>
       </c>
       <c r="G90">
-        <v>6.093901290494126</v>
+        <v>6.09390129049413</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -4258,7 +4258,7 @@
         <v>587</v>
       </c>
       <c r="G91">
-        <v>6.093901290494126</v>
+        <v>6.09390129049413</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -4281,7 +4281,7 @@
         <v>587</v>
       </c>
       <c r="G92">
-        <v>6.107003714666651</v>
+        <v>6.107003714666653</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -4304,7 +4304,7 @@
         <v>587</v>
       </c>
       <c r="G93">
-        <v>5.897015101019204</v>
+        <v>5.897015101019206</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -4327,7 +4327,7 @@
         <v>587</v>
       </c>
       <c r="G94">
-        <v>5.872259256026822</v>
+        <v>5.872259256026825</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -4347,7 +4347,7 @@
         <v>587</v>
       </c>
       <c r="G95">
-        <v>6.375031127880537</v>
+        <v>6.375031127880541</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -4370,7 +4370,7 @@
         <v>587</v>
       </c>
       <c r="G96">
-        <v>5.848563642215386</v>
+        <v>5.848563642215388</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -4413,7 +4413,7 @@
         <v>587</v>
       </c>
       <c r="G98">
-        <v>6.10964872036567</v>
+        <v>6.109648720365672</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -4436,7 +4436,7 @@
         <v>587</v>
       </c>
       <c r="G99">
-        <v>5.901045143111609</v>
+        <v>5.901045143111612</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -4459,7 +4459,7 @@
         <v>587</v>
       </c>
       <c r="G100">
-        <v>5.660617121714197</v>
+        <v>5.660617121714199</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -4482,7 +4482,7 @@
         <v>587</v>
       </c>
       <c r="G101">
-        <v>5.996835569861003</v>
+        <v>5.996835569861005</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -4505,7 +4505,7 @@
         <v>587</v>
       </c>
       <c r="G102">
-        <v>6.107003714666651</v>
+        <v>6.107003714666653</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -4528,7 +4528,7 @@
         <v>587</v>
       </c>
       <c r="G103">
-        <v>5.95814052787357</v>
+        <v>5.958140527873574</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -4551,7 +4551,7 @@
         <v>587</v>
       </c>
       <c r="G104">
-        <v>5.832587199439161</v>
+        <v>5.832587199439163</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -4574,7 +4574,7 @@
         <v>587</v>
       </c>
       <c r="G105">
-        <v>6.338105301393234</v>
+        <v>6.338105301393237</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -4597,7 +4597,7 @@
         <v>587</v>
       </c>
       <c r="G106">
-        <v>5.966645547720989</v>
+        <v>5.966645547720993</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -4620,7 +4620,7 @@
         <v>587</v>
       </c>
       <c r="G107">
-        <v>6.096671288336826</v>
+        <v>6.096671288336828</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -4643,7 +4643,7 @@
         <v>587</v>
       </c>
       <c r="G108">
-        <v>5.72176269675914</v>
+        <v>5.721762696759142</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -4666,7 +4666,7 @@
         <v>587</v>
       </c>
       <c r="G109">
-        <v>5.98433137901828</v>
+        <v>5.984331379018282</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -4689,7 +4689,7 @@
         <v>587</v>
       </c>
       <c r="G110">
-        <v>6.093901290494126</v>
+        <v>6.09390129049413</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -4712,7 +4712,7 @@
         <v>587</v>
       </c>
       <c r="G111">
-        <v>6.096671288336826</v>
+        <v>6.096671288336828</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -4735,7 +4735,7 @@
         <v>587</v>
       </c>
       <c r="G112">
-        <v>5.865786511413764</v>
+        <v>5.865786511413766</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -4847,7 +4847,7 @@
         <v>589</v>
       </c>
       <c r="G117">
-        <v>5.871458239791171</v>
+        <v>5.87145823979117</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -4916,7 +4916,7 @@
         <v>589</v>
       </c>
       <c r="G120">
-        <v>5.321099828563503</v>
+        <v>5.321099828563502</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -5097,7 +5097,7 @@
         <v>589</v>
       </c>
       <c r="G128">
-        <v>5.537811375660916</v>
+        <v>5.537811375660914</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -5166,7 +5166,7 @@
         <v>589</v>
       </c>
       <c r="G131">
-        <v>6.051403075804838</v>
+        <v>6.051403075804839</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -5465,7 +5465,7 @@
         <v>590</v>
       </c>
       <c r="G144">
-        <v>5.944092859691865</v>
+        <v>5.944092859691867</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -5511,7 +5511,7 @@
         <v>590</v>
       </c>
       <c r="G146">
-        <v>6.101254487164511</v>
+        <v>6.101254487164513</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -5534,7 +5534,7 @@
         <v>590</v>
       </c>
       <c r="G147">
-        <v>5.941447853992845</v>
+        <v>5.941447853992847</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -5554,7 +5554,7 @@
         <v>590</v>
       </c>
       <c r="G148">
-        <v>6.08582469143141</v>
+        <v>6.085824691431411</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -5577,7 +5577,7 @@
         <v>590</v>
       </c>
       <c r="G149">
-        <v>6.138599688727521</v>
+        <v>6.138599688727523</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -5600,7 +5600,7 @@
         <v>590</v>
       </c>
       <c r="G150">
-        <v>6.331995711160844</v>
+        <v>6.331995711160846</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -5620,7 +5620,7 @@
         <v>590</v>
       </c>
       <c r="G151">
-        <v>6.136141570515202</v>
+        <v>6.136141570515206</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -5643,7 +5643,7 @@
         <v>590</v>
       </c>
       <c r="G152">
-        <v>6.404107991946479</v>
+        <v>6.404107991946481</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -5666,7 +5666,7 @@
         <v>590</v>
       </c>
       <c r="G153">
-        <v>6.304812715737135</v>
+        <v>6.304812715737136</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -5686,7 +5686,7 @@
         <v>590</v>
       </c>
       <c r="G154">
-        <v>6.034356666895927</v>
+        <v>6.034356666895929</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -5706,7 +5706,7 @@
         <v>590</v>
       </c>
       <c r="G155">
-        <v>6.194641495689244</v>
+        <v>6.194641495689246</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -5752,7 +5752,7 @@
         <v>590</v>
       </c>
       <c r="G157">
-        <v>6.050351104817628</v>
+        <v>6.05035110481763</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -5775,7 +5775,7 @@
         <v>590</v>
       </c>
       <c r="G158">
-        <v>6.184236914412177</v>
+        <v>6.184236914412181</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -5798,7 +5798,7 @@
         <v>590</v>
       </c>
       <c r="G159">
-        <v>6.162033223865826</v>
+        <v>6.162033223865829</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -5818,7 +5818,7 @@
         <v>590</v>
       </c>
       <c r="G160">
-        <v>5.767373643460206</v>
+        <v>5.767373643460208</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -5841,7 +5841,7 @@
         <v>590</v>
       </c>
       <c r="G161">
-        <v>5.944092859691865</v>
+        <v>5.944092859691867</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -5861,7 +5861,7 @@
         <v>590</v>
       </c>
       <c r="G162">
-        <v>5.910081208977487</v>
+        <v>5.91008120897749</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -5884,7 +5884,7 @@
         <v>590</v>
       </c>
       <c r="G163">
-        <v>5.945286232545969</v>
+        <v>5.94528623254597</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -5907,7 +5907,7 @@
         <v>590</v>
       </c>
       <c r="G164">
-        <v>5.944092859691865</v>
+        <v>5.944092859691867</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -5930,7 +5930,7 @@
         <v>590</v>
       </c>
       <c r="G165">
-        <v>5.972203179688285</v>
+        <v>5.972203179688287</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -5953,7 +5953,7 @@
         <v>590</v>
       </c>
       <c r="G166">
-        <v>6.449529668985195</v>
+        <v>6.449529668985197</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -5976,7 +5976,7 @@
         <v>590</v>
       </c>
       <c r="G167">
-        <v>5.928345429820321</v>
+        <v>5.928345429820323</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -5999,7 +5999,7 @@
         <v>590</v>
       </c>
       <c r="G168">
-        <v>6.226687290900379</v>
+        <v>6.22668729090038</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -6022,7 +6022,7 @@
         <v>590</v>
       </c>
       <c r="G169">
-        <v>5.941447853992845</v>
+        <v>5.941447853992847</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -6042,7 +6042,7 @@
         <v>591</v>
       </c>
       <c r="G170">
-        <v>6.371269215507165</v>
+        <v>6.371269215507168</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -6062,7 +6062,7 @@
         <v>591</v>
       </c>
       <c r="G171">
-        <v>6.08701328311986</v>
+        <v>6.087013283119862</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -6085,7 +6085,7 @@
         <v>591</v>
       </c>
       <c r="G172">
-        <v>6.426025989141764</v>
+        <v>6.426025989141766</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -6108,7 +6108,7 @@
         <v>591</v>
       </c>
       <c r="G173">
-        <v>6.274029598364089</v>
+        <v>6.27402959836409</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -6131,7 +6131,7 @@
         <v>591</v>
       </c>
       <c r="G174">
-        <v>5.903226739810248</v>
+        <v>5.90322673981025</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -6154,7 +6154,7 @@
         <v>591</v>
       </c>
       <c r="G175">
-        <v>6.070963857171125</v>
+        <v>6.070963857171127</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -6200,7 +6200,7 @@
         <v>591</v>
       </c>
       <c r="G177">
-        <v>6.163513733345337</v>
+        <v>6.163513733345339</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -6223,7 +6223,7 @@
         <v>591</v>
       </c>
       <c r="G178">
-        <v>6.817477547318069</v>
+        <v>6.817477547318073</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -6246,7 +6246,7 @@
         <v>591</v>
       </c>
       <c r="G179">
-        <v>6.496836408867158</v>
+        <v>6.49683640886716</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -6266,7 +6266,7 @@
         <v>591</v>
       </c>
       <c r="G180">
-        <v>6.201237159048232</v>
+        <v>6.201237159048234</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -6289,7 +6289,7 @@
         <v>591</v>
       </c>
       <c r="G181">
-        <v>6.117062225542866</v>
+        <v>6.117062225542868</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -6309,7 +6309,7 @@
         <v>591</v>
       </c>
       <c r="G182">
-        <v>6.437805256429148</v>
+        <v>6.43780525642915</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -6329,7 +6329,7 @@
         <v>591</v>
       </c>
       <c r="G183">
-        <v>6.219557910752399</v>
+        <v>6.219557910752401</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -6352,7 +6352,7 @@
         <v>591</v>
       </c>
       <c r="G184">
-        <v>6.22418569409724</v>
+        <v>6.224185694097243</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -6398,7 +6398,7 @@
         <v>591</v>
       </c>
       <c r="G186">
-        <v>6.024982972882083</v>
+        <v>6.024982972882085</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -6421,7 +6421,7 @@
         <v>591</v>
       </c>
       <c r="G187">
-        <v>6.731370745667197</v>
+        <v>6.731370745667198</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -6582,7 +6582,7 @@
         <v>592</v>
       </c>
       <c r="G194">
-        <v>5.552562701535776</v>
+        <v>5.552562701535774</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -6605,7 +6605,7 @@
         <v>592</v>
       </c>
       <c r="G195">
-        <v>5.824579509948545</v>
+        <v>5.824579509948543</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -6628,7 +6628,7 @@
         <v>592</v>
       </c>
       <c r="G196">
-        <v>5.655976741086161</v>
+        <v>5.655976741086159</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -6651,7 +6651,7 @@
         <v>592</v>
       </c>
       <c r="G197">
-        <v>5.620363487686645</v>
+        <v>5.620363487686643</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -6674,7 +6674,7 @@
         <v>592</v>
       </c>
       <c r="G198">
-        <v>5.688818747327988</v>
+        <v>5.688818747327987</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -6720,7 +6720,7 @@
         <v>592</v>
       </c>
       <c r="G200">
-        <v>5.824579509948545</v>
+        <v>5.824579509948543</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -6743,7 +6743,7 @@
         <v>592</v>
       </c>
       <c r="G201">
-        <v>5.761714947717292</v>
+        <v>5.76171494771729</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -6766,7 +6766,7 @@
         <v>592</v>
       </c>
       <c r="G202">
-        <v>5.701796179356834</v>
+        <v>5.701796179356832</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -6789,7 +6789,7 @@
         <v>592</v>
       </c>
       <c r="G203">
-        <v>5.68604874948529</v>
+        <v>5.686048749485288</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -6812,7 +6812,7 @@
         <v>592</v>
       </c>
       <c r="G204">
-        <v>5.609389109458308</v>
+        <v>5.609389109458307</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -6858,7 +6858,7 @@
         <v>592</v>
       </c>
       <c r="G206">
-        <v>5.665292614797584</v>
+        <v>5.665292614797582</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -6904,7 +6904,7 @@
         <v>592</v>
       </c>
       <c r="G208">
-        <v>5.662360106566592</v>
+        <v>5.662360106566591</v>
       </c>
     </row>
     <row r="209" spans="1:7">
@@ -6927,7 +6927,7 @@
         <v>592</v>
       </c>
       <c r="G209">
-        <v>5.840326939820089</v>
+        <v>5.840326939820087</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -6950,7 +6950,7 @@
         <v>592</v>
       </c>
       <c r="G210">
-        <v>5.639872005481842</v>
+        <v>5.63987200548184</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -6973,7 +6973,7 @@
         <v>592</v>
       </c>
       <c r="G211">
-        <v>5.840326939820089</v>
+        <v>5.840326939820087</v>
       </c>
     </row>
     <row r="212" spans="1:7">
@@ -6996,7 +6996,7 @@
         <v>592</v>
       </c>
       <c r="G212">
-        <v>5.681040044669127</v>
+        <v>5.681040044669126</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -7019,7 +7019,7 @@
         <v>592</v>
       </c>
       <c r="G213">
-        <v>5.722817334776129</v>
+        <v>5.722817334776127</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -7062,7 +7062,7 @@
         <v>593</v>
       </c>
       <c r="G215">
-        <v>6.1476613536657</v>
+        <v>6.147661353665703</v>
       </c>
     </row>
     <row r="216" spans="1:7">
@@ -7085,7 +7085,7 @@
         <v>593</v>
       </c>
       <c r="G216">
-        <v>5.840269304642638</v>
+        <v>5.84026930464264</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -7108,7 +7108,7 @@
         <v>593</v>
       </c>
       <c r="G217">
-        <v>6.091011844801593</v>
+        <v>6.091011844801597</v>
       </c>
     </row>
     <row r="218" spans="1:7">
@@ -7131,7 +7131,7 @@
         <v>593</v>
       </c>
       <c r="G218">
-        <v>6.052829167060779</v>
+        <v>6.052829167060781</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -7154,7 +7154,7 @@
         <v>593</v>
       </c>
       <c r="G219">
-        <v>5.940659404528183</v>
+        <v>5.940659404528184</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -7177,7 +7177,7 @@
         <v>593</v>
       </c>
       <c r="G220">
-        <v>6.041099352183099</v>
+        <v>6.041099352183102</v>
       </c>
     </row>
     <row r="221" spans="1:7">
@@ -7200,7 +7200,7 @@
         <v>593</v>
       </c>
       <c r="G221">
-        <v>6.351308047715583</v>
+        <v>6.351308047715587</v>
       </c>
     </row>
     <row r="222" spans="1:7">
@@ -7223,7 +7223,7 @@
         <v>593</v>
       </c>
       <c r="G222">
-        <v>5.806118188794696</v>
+        <v>5.806118188794698</v>
       </c>
     </row>
     <row r="223" spans="1:7">
@@ -7246,7 +7246,7 @@
         <v>593</v>
       </c>
       <c r="G223">
-        <v>6.342215543403431</v>
+        <v>6.342215543403435</v>
       </c>
     </row>
     <row r="224" spans="1:7">
@@ -7269,7 +7269,7 @@
         <v>593</v>
       </c>
       <c r="G224">
-        <v>6.211496347621167</v>
+        <v>6.21149634762117</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -7292,7 +7292,7 @@
         <v>593</v>
       </c>
       <c r="G225">
-        <v>5.970423622555761</v>
+        <v>5.970423622555765</v>
       </c>
     </row>
     <row r="226" spans="1:7">
@@ -7315,7 +7315,7 @@
         <v>593</v>
       </c>
       <c r="G226">
-        <v>6.173012317975044</v>
+        <v>6.173012317975048</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -7338,7 +7338,7 @@
         <v>593</v>
       </c>
       <c r="G227">
-        <v>6.216419064135793</v>
+        <v>6.216419064135796</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -7361,7 +7361,7 @@
         <v>593</v>
       </c>
       <c r="G228">
-        <v>6.236175970327582</v>
+        <v>6.236175970327584</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -7384,7 +7384,7 @@
         <v>593</v>
       </c>
       <c r="G229">
-        <v>5.701132088382498</v>
+        <v>5.7011320883825</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -7407,7 +7407,7 @@
         <v>593</v>
       </c>
       <c r="G230">
-        <v>6.125475925783266</v>
+        <v>6.125475925783269</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -7430,7 +7430,7 @@
         <v>593</v>
       </c>
       <c r="G231">
-        <v>6.117327282608794</v>
+        <v>6.117327282608795</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -7453,7 +7453,7 @@
         <v>593</v>
       </c>
       <c r="G232">
-        <v>6.054781959168458</v>
+        <v>6.05478195916846</v>
       </c>
     </row>
     <row r="233" spans="1:7">
@@ -7476,7 +7476,7 @@
         <v>593</v>
       </c>
       <c r="G233">
-        <v>6.124065576128898</v>
+        <v>6.124065576128902</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -7499,7 +7499,7 @@
         <v>593</v>
       </c>
       <c r="G234">
-        <v>5.981398000525441</v>
+        <v>5.981398000525444</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -7522,7 +7522,7 @@
         <v>593</v>
       </c>
       <c r="G235">
-        <v>6.451267211755657</v>
+        <v>6.451267211755661</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -7568,7 +7568,7 @@
         <v>594</v>
       </c>
       <c r="G237">
-        <v>5.889588489177782</v>
+        <v>5.889588489177778</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -7591,7 +7591,7 @@
         <v>594</v>
       </c>
       <c r="G238">
-        <v>6.154760631724746</v>
+        <v>6.154760631724744</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -7614,7 +7614,7 @@
         <v>594</v>
       </c>
       <c r="G239">
-        <v>6.067992182436478</v>
+        <v>6.067992182436476</v>
       </c>
     </row>
     <row r="240" spans="1:7">
@@ -7637,7 +7637,7 @@
         <v>594</v>
       </c>
       <c r="G240">
-        <v>5.802230065488815</v>
+        <v>5.802230065488813</v>
       </c>
     </row>
     <row r="241" spans="1:7">
@@ -7683,7 +7683,7 @@
         <v>594</v>
       </c>
       <c r="G242">
-        <v>6.403264657618425</v>
+        <v>6.403264657618423</v>
       </c>
     </row>
     <row r="243" spans="1:7">
@@ -7706,7 +7706,7 @@
         <v>595</v>
       </c>
       <c r="G243">
-        <v>6.403264657618425</v>
+        <v>6.403264657618423</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -7729,7 +7729,7 @@
         <v>594</v>
       </c>
       <c r="G244">
-        <v>5.909910588669542</v>
+        <v>5.909910588669539</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -7752,7 +7752,7 @@
         <v>594</v>
       </c>
       <c r="G245">
-        <v>6.230031075429442</v>
+        <v>6.23003107542944</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -7821,7 +7821,7 @@
         <v>594</v>
       </c>
       <c r="G248">
-        <v>5.874130384039133</v>
+        <v>5.874130384039131</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -7844,7 +7844,7 @@
         <v>594</v>
       </c>
       <c r="G249">
-        <v>5.698146234151328</v>
+        <v>5.698146234151326</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -7936,7 +7936,7 @@
         <v>594</v>
       </c>
       <c r="G253">
-        <v>5.970051011526931</v>
+        <v>5.970051011526929</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -7959,7 +7959,7 @@
         <v>594</v>
       </c>
       <c r="G254">
-        <v>6.105732541442172</v>
+        <v>6.105732541442168</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -7979,7 +7979,7 @@
         <v>594</v>
       </c>
       <c r="G255">
-        <v>5.733600197110666</v>
+        <v>5.733600197110662</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -8002,7 +8002,7 @@
         <v>594</v>
       </c>
       <c r="G256">
-        <v>6.258913095307066</v>
+        <v>6.258913095307064</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -8025,7 +8025,7 @@
         <v>594</v>
       </c>
       <c r="G257">
-        <v>5.663753549193294</v>
+        <v>5.663753549193291</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -8068,7 +8068,7 @@
         <v>596</v>
       </c>
       <c r="G259">
-        <v>6.468019281757095</v>
+        <v>6.468019281757099</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -8114,7 +8114,7 @@
         <v>596</v>
       </c>
       <c r="G261">
-        <v>6.506142781805553</v>
+        <v>6.506142781805555</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -8137,7 +8137,7 @@
         <v>596</v>
       </c>
       <c r="G262">
-        <v>6.148519779690971</v>
+        <v>6.148519779690973</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -8183,7 +8183,7 @@
         <v>596</v>
       </c>
       <c r="G264">
-        <v>6.432259780018872</v>
+        <v>6.432259780018874</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -8206,7 +8206,7 @@
         <v>596</v>
       </c>
       <c r="G265">
-        <v>6.020748487361124</v>
+        <v>6.020748487361126</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -8229,7 +8229,7 @@
         <v>596</v>
       </c>
       <c r="G266">
-        <v>6.308512089219083</v>
+        <v>6.308512089219085</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -8275,7 +8275,7 @@
         <v>596</v>
       </c>
       <c r="G268">
-        <v>5.974332916953315</v>
+        <v>5.974332916953311</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -8298,7 +8298,7 @@
         <v>595</v>
       </c>
       <c r="G269">
-        <v>5.974332916953315</v>
+        <v>5.974332916953311</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -8321,7 +8321,7 @@
         <v>596</v>
       </c>
       <c r="G270">
-        <v>6.098607287072476</v>
+        <v>6.098607287072478</v>
       </c>
     </row>
     <row r="271" spans="1:7">
@@ -8427,7 +8427,7 @@
         <v>596</v>
       </c>
       <c r="G275">
-        <v>6.098607287072476</v>
+        <v>6.098607287072478</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -8496,7 +8496,7 @@
         <v>596</v>
       </c>
       <c r="G278">
-        <v>5.996818777006289</v>
+        <v>5.996818777006291</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -8519,7 +8519,7 @@
         <v>596</v>
       </c>
       <c r="G279">
-        <v>6.247470473865556</v>
+        <v>6.247470473865559</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -8542,7 +8542,7 @@
         <v>596</v>
       </c>
       <c r="G280">
-        <v>6.13828468970203</v>
+        <v>6.138284689702032</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -8585,7 +8585,7 @@
         <v>596</v>
       </c>
       <c r="G282">
-        <v>6.098607287072476</v>
+        <v>6.098607287072478</v>
       </c>
     </row>
     <row r="283" spans="1:7">
@@ -8608,7 +8608,7 @@
         <v>596</v>
       </c>
       <c r="G283">
-        <v>6.250115479564577</v>
+        <v>6.250115479564578</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -8631,7 +8631,7 @@
         <v>596</v>
       </c>
       <c r="G284">
-        <v>5.786901924035569</v>
+        <v>5.786901924035571</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -8654,7 +8654,7 @@
         <v>596</v>
       </c>
       <c r="G285">
-        <v>6.157759111132086</v>
+        <v>6.157759111132088</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -8677,7 +8677,7 @@
         <v>596</v>
       </c>
       <c r="G286">
-        <v>6.098607287072476</v>
+        <v>6.098607287072478</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -8700,7 +8700,7 @@
         <v>596</v>
       </c>
       <c r="G287">
-        <v>6.17905383962139</v>
+        <v>6.179053839621392</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -8723,7 +8723,7 @@
         <v>596</v>
       </c>
       <c r="G288">
-        <v>6.098607287072476</v>
+        <v>6.098607287072478</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -8743,7 +8743,7 @@
         <v>596</v>
       </c>
       <c r="G289">
-        <v>6.15141950845084</v>
+        <v>6.151419508450842</v>
       </c>
     </row>
     <row r="290" spans="1:7">
@@ -8766,7 +8766,7 @@
         <v>596</v>
       </c>
       <c r="G290">
-        <v>6.230058370273464</v>
+        <v>6.230058370273466</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -8789,7 +8789,7 @@
         <v>596</v>
       </c>
       <c r="G291">
-        <v>6.098607287072476</v>
+        <v>6.098607287072478</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -8812,7 +8812,7 @@
         <v>596</v>
       </c>
       <c r="G292">
-        <v>6.527553829498285</v>
+        <v>6.527553829498287</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -8835,7 +8835,7 @@
         <v>596</v>
       </c>
       <c r="G293">
-        <v>6.108939713402301</v>
+        <v>6.108939713402303</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -8898,7 +8898,7 @@
         <v>596</v>
       </c>
       <c r="G296">
-        <v>6.098607287072476</v>
+        <v>6.098607287072478</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -8990,7 +8990,7 @@
         <v>596</v>
       </c>
       <c r="G300">
-        <v>6.097139150548677</v>
+        <v>6.097139150548679</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -9010,7 +9010,7 @@
         <v>597</v>
       </c>
       <c r="G301">
-        <v>5.910997391655846</v>
+        <v>5.91099739165585</v>
       </c>
     </row>
     <row r="302" spans="1:7">
@@ -9033,7 +9033,7 @@
         <v>597</v>
       </c>
       <c r="G302">
-        <v>5.837412807116547</v>
+        <v>5.837412807116549</v>
       </c>
     </row>
     <row r="303" spans="1:7">
@@ -9056,7 +9056,7 @@
         <v>597</v>
       </c>
       <c r="G303">
-        <v>6.013671720544719</v>
+        <v>6.013671720544722</v>
       </c>
     </row>
     <row r="304" spans="1:7">
@@ -9076,7 +9076,7 @@
         <v>597</v>
       </c>
       <c r="G304">
-        <v>5.402175221830102</v>
+        <v>5.402175221830103</v>
       </c>
     </row>
     <row r="305" spans="1:7">
@@ -9099,7 +9099,7 @@
         <v>597</v>
       </c>
       <c r="G305">
-        <v>5.866733730851158</v>
+        <v>5.866733730851162</v>
       </c>
     </row>
     <row r="306" spans="1:7">
@@ -9122,7 +9122,7 @@
         <v>597</v>
       </c>
       <c r="G306">
-        <v>5.633406910523273</v>
+        <v>5.633406910523276</v>
       </c>
     </row>
     <row r="307" spans="1:7">
@@ -9145,7 +9145,7 @@
         <v>597</v>
       </c>
       <c r="G307">
-        <v>6.41449647307054</v>
+        <v>6.414496473070545</v>
       </c>
     </row>
     <row r="308" spans="1:7">
@@ -9168,7 +9168,7 @@
         <v>597</v>
       </c>
       <c r="G308">
-        <v>5.753449499161092</v>
+        <v>5.753449499161095</v>
       </c>
     </row>
     <row r="309" spans="1:7">
@@ -9191,7 +9191,7 @@
         <v>597</v>
       </c>
       <c r="G309">
-        <v>5.82446257080441</v>
+        <v>5.824462570804413</v>
       </c>
     </row>
     <row r="310" spans="1:7">
@@ -9214,7 +9214,7 @@
         <v>597</v>
       </c>
       <c r="G310">
-        <v>5.788833648078586</v>
+        <v>5.788833648078589</v>
       </c>
     </row>
     <row r="311" spans="1:7">
@@ -9237,7 +9237,7 @@
         <v>597</v>
       </c>
       <c r="G311">
-        <v>6.026486420329019</v>
+        <v>6.026486420329021</v>
       </c>
     </row>
     <row r="312" spans="1:7">
@@ -9260,7 +9260,7 @@
         <v>597</v>
       </c>
       <c r="G312">
-        <v>5.815254014343156</v>
+        <v>5.81525401434316</v>
       </c>
     </row>
     <row r="313" spans="1:7">
@@ -9283,7 +9283,7 @@
         <v>597</v>
       </c>
       <c r="G313">
-        <v>6.118112227338519</v>
+        <v>6.118112227338524</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -9306,7 +9306,7 @@
         <v>597</v>
       </c>
       <c r="G314">
-        <v>5.892534577793948</v>
+        <v>5.892534577793952</v>
       </c>
     </row>
     <row r="315" spans="1:7">
@@ -9329,7 +9329,7 @@
         <v>597</v>
       </c>
       <c r="G315">
-        <v>5.50569004004305</v>
+        <v>5.505690040043052</v>
       </c>
     </row>
     <row r="316" spans="1:7">
@@ -9352,7 +9352,7 @@
         <v>597</v>
       </c>
       <c r="G316">
-        <v>5.644604052640797</v>
+        <v>5.6446040526408</v>
       </c>
     </row>
     <row r="317" spans="1:7">
@@ -9375,7 +9375,7 @@
         <v>597</v>
       </c>
       <c r="G317">
-        <v>6.085830905768453</v>
+        <v>6.085830905768456</v>
       </c>
     </row>
     <row r="318" spans="1:7">
@@ -9398,7 +9398,7 @@
         <v>597</v>
       </c>
       <c r="G318">
-        <v>5.530463789724622</v>
+        <v>5.530463789724624</v>
       </c>
     </row>
     <row r="319" spans="1:7">
@@ -9421,7 +9421,7 @@
         <v>597</v>
       </c>
       <c r="G319">
-        <v>6.10734593138615</v>
+        <v>6.107345931386154</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -9444,7 +9444,7 @@
         <v>597</v>
       </c>
       <c r="G320">
-        <v>5.433983669806154</v>
+        <v>5.433983669806156</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -9464,7 +9464,7 @@
         <v>597</v>
       </c>
       <c r="G321">
-        <v>5.297948143515902</v>
+        <v>5.297948143515904</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -9484,7 +9484,7 @@
         <v>598</v>
       </c>
       <c r="G322">
-        <v>5.670401150825465</v>
+        <v>5.670401150825463</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -9599,7 +9599,7 @@
         <v>598</v>
       </c>
       <c r="G327">
-        <v>5.75907669203433</v>
+        <v>5.759076692034328</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -9622,7 +9622,7 @@
         <v>598</v>
       </c>
       <c r="G328">
-        <v>5.862940666016629</v>
+        <v>5.862940666016628</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -9691,7 +9691,7 @@
         <v>598</v>
       </c>
       <c r="G331">
-        <v>5.58205246521804</v>
+        <v>5.582052465218038</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -9806,7 +9806,7 @@
         <v>598</v>
       </c>
       <c r="G336">
-        <v>5.670339218746828</v>
+        <v>5.670339218746826</v>
       </c>
     </row>
     <row r="337" spans="1:7">
@@ -9829,7 +9829,7 @@
         <v>598</v>
       </c>
       <c r="G337">
-        <v>5.861967812923143</v>
+        <v>5.861967812923145</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -9852,7 +9852,7 @@
         <v>598</v>
       </c>
       <c r="G338">
-        <v>5.830083323373954</v>
+        <v>5.830083323373956</v>
       </c>
     </row>
     <row r="339" spans="1:7">
@@ -9895,7 +9895,7 @@
         <v>598</v>
       </c>
       <c r="G340">
-        <v>5.619025794878783</v>
+        <v>5.619025794878781</v>
       </c>
     </row>
     <row r="341" spans="1:7">
@@ -10102,7 +10102,7 @@
         <v>598</v>
       </c>
       <c r="G349">
-        <v>5.589757056067627</v>
+        <v>5.589757056067625</v>
       </c>
     </row>
     <row r="350" spans="1:7">
@@ -10148,7 +10148,7 @@
         <v>598</v>
       </c>
       <c r="G351">
-        <v>5.698772319566699</v>
+        <v>5.698772319566697</v>
       </c>
     </row>
     <row r="352" spans="1:7">
@@ -10217,7 +10217,7 @@
         <v>599</v>
       </c>
       <c r="G354">
-        <v>5.799807121726762</v>
+        <v>5.799807121726764</v>
       </c>
     </row>
     <row r="355" spans="1:7">
@@ -10263,7 +10263,7 @@
         <v>599</v>
       </c>
       <c r="G356">
-        <v>6.047626260628863</v>
+        <v>6.047626260628864</v>
       </c>
     </row>
     <row r="357" spans="1:7">
@@ -10332,7 +10332,7 @@
         <v>599</v>
       </c>
       <c r="G359">
-        <v>5.768269354251893</v>
+        <v>5.768269354251895</v>
       </c>
     </row>
     <row r="360" spans="1:7">
@@ -10355,7 +10355,7 @@
         <v>586</v>
       </c>
       <c r="G360">
-        <v>5.768269354251893</v>
+        <v>5.768269354251895</v>
       </c>
     </row>
     <row r="361" spans="1:7">
@@ -10378,7 +10378,7 @@
         <v>599</v>
       </c>
       <c r="G361">
-        <v>5.726110225112982</v>
+        <v>5.726110225112984</v>
       </c>
     </row>
     <row r="362" spans="1:7">
@@ -10424,7 +10424,7 @@
         <v>599</v>
       </c>
       <c r="G363">
-        <v>6.048100873021101</v>
+        <v>6.048100873021103</v>
       </c>
     </row>
     <row r="364" spans="1:7">
@@ -10470,7 +10470,7 @@
         <v>599</v>
       </c>
       <c r="G365">
-        <v>5.774727959121699</v>
+        <v>5.774727959121701</v>
       </c>
     </row>
     <row r="366" spans="1:7">
@@ -10516,7 +10516,7 @@
         <v>599</v>
       </c>
       <c r="G367">
-        <v>5.66151671073347</v>
+        <v>5.661516710733472</v>
       </c>
     </row>
     <row r="368" spans="1:7">
@@ -10539,7 +10539,7 @@
         <v>599</v>
       </c>
       <c r="G368">
-        <v>5.968940211990851</v>
+        <v>5.968940211990852</v>
       </c>
     </row>
     <row r="369" spans="1:7">
@@ -10562,7 +10562,7 @@
         <v>599</v>
       </c>
       <c r="G369">
-        <v>5.801054738619272</v>
+        <v>5.801054738619274</v>
       </c>
     </row>
     <row r="370" spans="1:7">
@@ -10608,7 +10608,7 @@
         <v>599</v>
       </c>
       <c r="G371">
-        <v>6.142783848061028</v>
+        <v>6.14278384806103</v>
       </c>
     </row>
     <row r="372" spans="1:7">
@@ -10654,7 +10654,7 @@
         <v>599</v>
       </c>
       <c r="G373">
-        <v>6.058433299350926</v>
+        <v>6.058433299350928</v>
       </c>
     </row>
     <row r="374" spans="1:7">
@@ -10677,7 +10677,7 @@
         <v>599</v>
       </c>
       <c r="G374">
-        <v>5.7693542386412</v>
+        <v>5.769354238641202</v>
       </c>
     </row>
     <row r="375" spans="1:7">
@@ -10746,7 +10746,7 @@
         <v>599</v>
       </c>
       <c r="G377">
-        <v>5.888810434909785</v>
+        <v>5.888810434909787</v>
       </c>
     </row>
     <row r="378" spans="1:7">
@@ -10815,7 +10815,7 @@
         <v>599</v>
       </c>
       <c r="G380">
-        <v>6.047663376718876</v>
+        <v>6.047663376718877</v>
       </c>
     </row>
     <row r="381" spans="1:7">
@@ -10838,7 +10838,7 @@
         <v>599</v>
       </c>
       <c r="G381">
-        <v>6.083984325446218</v>
+        <v>6.083984325446219</v>
       </c>
     </row>
     <row r="382" spans="1:7">
@@ -10858,7 +10858,7 @@
         <v>600</v>
       </c>
       <c r="G382">
-        <v>6.28380205932197</v>
+        <v>6.283802059321974</v>
       </c>
     </row>
     <row r="383" spans="1:7">
@@ -10881,7 +10881,7 @@
         <v>600</v>
       </c>
       <c r="G383">
-        <v>6.05389013575105</v>
+        <v>6.053890135751051</v>
       </c>
     </row>
     <row r="384" spans="1:7">
@@ -10901,7 +10901,7 @@
         <v>600</v>
       </c>
       <c r="G384">
-        <v>6.203253219122765</v>
+        <v>6.203253219122767</v>
       </c>
     </row>
     <row r="385" spans="1:7">
@@ -10924,7 +10924,7 @@
         <v>600</v>
       </c>
       <c r="G385">
-        <v>6.15560372518854</v>
+        <v>6.155603725188544</v>
       </c>
     </row>
     <row r="386" spans="1:7">
@@ -10990,7 +10990,7 @@
         <v>600</v>
       </c>
       <c r="G388">
-        <v>5.869128387116615</v>
+        <v>5.869128387116617</v>
       </c>
     </row>
     <row r="389" spans="1:7">
@@ -11036,7 +11036,7 @@
         <v>600</v>
       </c>
       <c r="G390">
-        <v>6.190279513839431</v>
+        <v>6.190279513839434</v>
       </c>
     </row>
     <row r="391" spans="1:7">
@@ -11059,7 +11059,7 @@
         <v>600</v>
       </c>
       <c r="G391">
-        <v>6.310096011768681</v>
+        <v>6.310096011768684</v>
       </c>
     </row>
     <row r="392" spans="1:7">
@@ -11082,7 +11082,7 @@
         <v>600</v>
       </c>
       <c r="G392">
-        <v>6.332714042785528</v>
+        <v>6.332714042785532</v>
       </c>
     </row>
     <row r="393" spans="1:7">
@@ -11105,7 +11105,7 @@
         <v>600</v>
       </c>
       <c r="G393">
-        <v>6.337692194067576</v>
+        <v>6.337692194067578</v>
       </c>
     </row>
     <row r="394" spans="1:7">
@@ -11174,7 +11174,7 @@
         <v>600</v>
       </c>
       <c r="G396">
-        <v>6.107935171743912</v>
+        <v>6.107935171743914</v>
       </c>
     </row>
     <row r="397" spans="1:7">
@@ -11197,7 +11197,7 @@
         <v>600</v>
       </c>
       <c r="G397">
-        <v>6.269073233567583</v>
+        <v>6.269073233567585</v>
       </c>
     </row>
     <row r="398" spans="1:7">
@@ -11220,7 +11220,7 @@
         <v>600</v>
       </c>
       <c r="G398">
-        <v>6.07240296749337</v>
+        <v>6.072402967493374</v>
       </c>
     </row>
     <row r="399" spans="1:7">
@@ -11243,7 +11243,7 @@
         <v>600</v>
       </c>
       <c r="G399">
-        <v>6.303397286022126</v>
+        <v>6.303397286022128</v>
       </c>
     </row>
     <row r="400" spans="1:7">
@@ -11266,7 +11266,7 @@
         <v>600</v>
       </c>
       <c r="G400">
-        <v>6.03802337190998</v>
+        <v>6.038023371909982</v>
       </c>
     </row>
     <row r="401" spans="1:7">
@@ -11289,7 +11289,7 @@
         <v>600</v>
       </c>
       <c r="G401">
-        <v>5.807888402949447</v>
+        <v>5.807888402949449</v>
       </c>
     </row>
     <row r="402" spans="1:7">
@@ -11312,7 +11312,7 @@
         <v>600</v>
       </c>
       <c r="G402">
-        <v>5.726909019626253</v>
+        <v>5.726909019626254</v>
       </c>
     </row>
     <row r="403" spans="1:7">
@@ -11381,7 +11381,7 @@
         <v>600</v>
       </c>
       <c r="G405">
-        <v>6.043539454846848</v>
+        <v>6.04353945484685</v>
       </c>
     </row>
     <row r="406" spans="1:7">
@@ -11404,7 +11404,7 @@
         <v>600</v>
       </c>
       <c r="G406">
-        <v>6.145105023653817</v>
+        <v>6.145105023653818</v>
       </c>
     </row>
     <row r="407" spans="1:7">
@@ -11427,7 +11427,7 @@
         <v>600</v>
       </c>
       <c r="G407">
-        <v>5.777157622791298</v>
+        <v>5.777157622791299</v>
       </c>
     </row>
     <row r="408" spans="1:7">
@@ -11450,7 +11450,7 @@
         <v>600</v>
       </c>
       <c r="G408">
-        <v>6.086193998196097</v>
+        <v>6.086193998196101</v>
       </c>
     </row>
     <row r="409" spans="1:7">
@@ -11473,7 +11473,7 @@
         <v>600</v>
       </c>
       <c r="G409">
-        <v>6.132617435734471</v>
+        <v>6.132617435734473</v>
       </c>
     </row>
     <row r="410" spans="1:7">
@@ -11493,7 +11493,7 @@
         <v>600</v>
       </c>
       <c r="G410">
-        <v>5.872115361630249</v>
+        <v>5.872115361630251</v>
       </c>
     </row>
     <row r="411" spans="1:7">
@@ -11536,7 +11536,7 @@
         <v>600</v>
       </c>
       <c r="G412">
-        <v>6.15560372518854</v>
+        <v>6.155603725188544</v>
       </c>
     </row>
     <row r="413" spans="1:7">
@@ -11559,7 +11559,7 @@
         <v>600</v>
       </c>
       <c r="G413">
-        <v>6.158248730887562</v>
+        <v>6.158248730887563</v>
       </c>
     </row>
     <row r="414" spans="1:7">
@@ -11579,7 +11579,7 @@
         <v>601</v>
       </c>
       <c r="G414">
-        <v>5.812401194707403</v>
+        <v>5.812401194707401</v>
       </c>
     </row>
     <row r="415" spans="1:7">
@@ -11602,7 +11602,7 @@
         <v>601</v>
       </c>
       <c r="G415">
-        <v>6.36281385036146</v>
+        <v>6.362813850361458</v>
       </c>
     </row>
     <row r="416" spans="1:7">
@@ -11665,7 +11665,7 @@
         <v>601</v>
       </c>
       <c r="G418">
-        <v>6.42704747918586</v>
+        <v>6.427047479185862</v>
       </c>
     </row>
     <row r="419" spans="1:7">
@@ -11708,7 +11708,7 @@
         <v>601</v>
       </c>
       <c r="G420">
-        <v>6.657865050834675</v>
+        <v>6.657865050834674</v>
       </c>
     </row>
     <row r="421" spans="1:7">
@@ -11754,7 +11754,7 @@
         <v>601</v>
       </c>
       <c r="G422">
-        <v>6.291945671108272</v>
+        <v>6.29194567110827</v>
       </c>
     </row>
     <row r="423" spans="1:7">
@@ -11863,7 +11863,7 @@
         <v>601</v>
       </c>
       <c r="G427">
-        <v>6.194387883501229</v>
+        <v>6.194387883501228</v>
       </c>
     </row>
     <row r="428" spans="1:7">
@@ -11886,7 +11886,7 @@
         <v>601</v>
       </c>
       <c r="G428">
-        <v>5.922805425973892</v>
+        <v>5.92280542597389</v>
       </c>
     </row>
     <row r="429" spans="1:7">
@@ -11909,7 +11909,7 @@
         <v>601</v>
       </c>
       <c r="G429">
-        <v>5.899153802204906</v>
+        <v>5.899153802204904</v>
       </c>
     </row>
     <row r="430" spans="1:7">
@@ -12024,7 +12024,7 @@
         <v>601</v>
       </c>
       <c r="G434">
-        <v>5.88019843841523</v>
+        <v>5.880198438415229</v>
       </c>
     </row>
     <row r="435" spans="1:7">
@@ -12047,7 +12047,7 @@
         <v>601</v>
       </c>
       <c r="G435">
-        <v>6.370538308852587</v>
+        <v>6.370538308852589</v>
       </c>
     </row>
     <row r="436" spans="1:7">
@@ -12231,7 +12231,7 @@
         <v>602</v>
       </c>
       <c r="G443">
-        <v>5.910863232163011</v>
+        <v>5.910863232163009</v>
       </c>
     </row>
     <row r="444" spans="1:7">
@@ -12254,7 +12254,7 @@
         <v>602</v>
       </c>
       <c r="G444">
-        <v>6.224399416983535</v>
+        <v>6.224399416983537</v>
       </c>
     </row>
     <row r="445" spans="1:7">
@@ -12300,7 +12300,7 @@
         <v>602</v>
       </c>
       <c r="G446">
-        <v>6.128633557482478</v>
+        <v>6.12863355748248</v>
       </c>
     </row>
     <row r="447" spans="1:7">
@@ -12369,7 +12369,7 @@
         <v>602</v>
       </c>
       <c r="G449">
-        <v>5.80834517689046</v>
+        <v>5.808345176890461</v>
       </c>
     </row>
     <row r="450" spans="1:7">
@@ -12415,7 +12415,7 @@
         <v>602</v>
       </c>
       <c r="G451">
-        <v>6.455505522995705</v>
+        <v>6.455505522995707</v>
       </c>
     </row>
     <row r="452" spans="1:7">
@@ -12504,7 +12504,7 @@
         <v>602</v>
       </c>
       <c r="G455">
-        <v>6.047846623655805</v>
+        <v>6.047846623655807</v>
       </c>
     </row>
     <row r="456" spans="1:7">
@@ -12527,7 +12527,7 @@
         <v>602</v>
       </c>
       <c r="G456">
-        <v>6.042910399477532</v>
+        <v>6.042910399477534</v>
       </c>
     </row>
     <row r="457" spans="1:7">
@@ -12550,7 +12550,7 @@
         <v>602</v>
       </c>
       <c r="G457">
-        <v>5.729299219053474</v>
+        <v>5.729299219053476</v>
       </c>
     </row>
     <row r="458" spans="1:7">
@@ -12573,7 +12573,7 @@
         <v>602</v>
       </c>
       <c r="G458">
-        <v>6.042910399477532</v>
+        <v>6.042910399477534</v>
       </c>
     </row>
     <row r="459" spans="1:7">
@@ -12688,7 +12688,7 @@
         <v>602</v>
       </c>
       <c r="G463">
-        <v>6.042910399477532</v>
+        <v>6.042910399477534</v>
       </c>
     </row>
     <row r="464" spans="1:7">
@@ -12734,7 +12734,7 @@
         <v>588</v>
       </c>
       <c r="G465">
-        <v>6.320994168672226</v>
+        <v>6.320994168672223</v>
       </c>
     </row>
     <row r="466" spans="1:7">
@@ -12757,7 +12757,7 @@
         <v>588</v>
       </c>
       <c r="G466">
-        <v>6.298654657057827</v>
+        <v>6.298654657057825</v>
       </c>
     </row>
     <row r="467" spans="1:7">
@@ -12780,7 +12780,7 @@
         <v>588</v>
       </c>
       <c r="G467">
-        <v>5.879996168190455</v>
+        <v>5.879996168190451</v>
       </c>
     </row>
     <row r="468" spans="1:7">
@@ -12803,7 +12803,7 @@
         <v>588</v>
       </c>
       <c r="G468">
-        <v>6.334112162718859</v>
+        <v>6.334112162718857</v>
       </c>
     </row>
     <row r="469" spans="1:7">
@@ -12849,7 +12849,7 @@
         <v>588</v>
       </c>
       <c r="G470">
-        <v>6.314403177892596</v>
+        <v>6.314403177892594</v>
       </c>
     </row>
     <row r="471" spans="1:7">
@@ -12872,7 +12872,7 @@
         <v>588</v>
       </c>
       <c r="G471">
-        <v>6.525708682954199</v>
+        <v>6.525708682954197</v>
       </c>
     </row>
     <row r="472" spans="1:7">
@@ -12895,7 +12895,7 @@
         <v>588</v>
       </c>
       <c r="G472">
-        <v>6.417545689781408</v>
+        <v>6.417545689781407</v>
       </c>
     </row>
     <row r="473" spans="1:7">
@@ -12918,7 +12918,7 @@
         <v>588</v>
       </c>
       <c r="G473">
-        <v>6.072798071663894</v>
+        <v>6.072798071663891</v>
       </c>
     </row>
     <row r="474" spans="1:7">
@@ -12941,7 +12941,7 @@
         <v>588</v>
       </c>
       <c r="G474">
-        <v>6.225115766354391</v>
+        <v>6.225115766354388</v>
       </c>
     </row>
     <row r="475" spans="1:7">
@@ -12964,7 +12964,7 @@
         <v>588</v>
       </c>
       <c r="G475">
-        <v>6.413199289323681</v>
+        <v>6.413199289323679</v>
       </c>
     </row>
     <row r="476" spans="1:7">
@@ -12987,7 +12987,7 @@
         <v>588</v>
       </c>
       <c r="G476">
-        <v>6.059820639635048</v>
+        <v>6.059820639635046</v>
       </c>
     </row>
     <row r="477" spans="1:7">
@@ -13010,7 +13010,7 @@
         <v>588</v>
       </c>
       <c r="G477">
-        <v>6.048858037486544</v>
+        <v>6.04885803748654</v>
       </c>
     </row>
     <row r="478" spans="1:7">
@@ -13030,7 +13030,7 @@
         <v>588</v>
       </c>
       <c r="G478">
-        <v>6.626921113516913</v>
+        <v>6.626921113516912</v>
       </c>
     </row>
     <row r="479" spans="1:7">
@@ -13053,7 +13053,7 @@
         <v>588</v>
       </c>
       <c r="G479">
-        <v>5.936708301076581</v>
+        <v>5.936708301076577</v>
       </c>
     </row>
     <row r="480" spans="1:7">
@@ -13076,7 +13076,7 @@
         <v>588</v>
       </c>
       <c r="G480">
-        <v>6.070153065964875</v>
+        <v>6.070153065964871</v>
       </c>
     </row>
     <row r="481" spans="1:7">
@@ -13099,7 +13099,7 @@
         <v>588</v>
       </c>
       <c r="G481">
-        <v>6.410266558719123</v>
+        <v>6.410266558719122</v>
       </c>
     </row>
     <row r="482" spans="1:7">
@@ -13122,7 +13122,7 @@
         <v>588</v>
       </c>
       <c r="G482">
-        <v>6.32749264069995</v>
+        <v>6.327492640699949</v>
       </c>
     </row>
     <row r="483" spans="1:7">
@@ -13145,7 +13145,7 @@
         <v>588</v>
       </c>
       <c r="G483">
-        <v>6.004187604437292</v>
+        <v>6.004187604437289</v>
       </c>
     </row>
     <row r="484" spans="1:7">
@@ -13168,7 +13168,7 @@
         <v>588</v>
       </c>
       <c r="G484">
-        <v>5.785200108584481</v>
+        <v>5.785200108584477</v>
       </c>
     </row>
     <row r="485" spans="1:7">
@@ -13191,7 +13191,7 @@
         <v>588</v>
       </c>
       <c r="G485">
-        <v>6.341167453951052</v>
+        <v>6.341167453951051</v>
       </c>
     </row>
     <row r="486" spans="1:7">
@@ -13214,7 +13214,7 @@
         <v>588</v>
       </c>
       <c r="G486">
-        <v>5.71311048634242</v>
+        <v>5.713110486342416</v>
       </c>
     </row>
     <row r="487" spans="1:7">
@@ -13237,7 +13237,7 @@
         <v>588</v>
       </c>
       <c r="G487">
-        <v>6.202199196926915</v>
+        <v>6.202199196926913</v>
       </c>
     </row>
     <row r="488" spans="1:7">
@@ -13260,7 +13260,7 @@
         <v>588</v>
       </c>
       <c r="G488">
-        <v>6.059820639635048</v>
+        <v>6.059820639635046</v>
       </c>
     </row>
     <row r="489" spans="1:7">
@@ -13283,7 +13283,7 @@
         <v>587</v>
       </c>
       <c r="G489">
-        <v>6.059820639635048</v>
+        <v>6.059820639635046</v>
       </c>
     </row>
     <row r="490" spans="1:7">
@@ -13306,7 +13306,7 @@
         <v>588</v>
       </c>
       <c r="G490">
-        <v>6.05705064179235</v>
+        <v>6.057050641792348</v>
       </c>
     </row>
     <row r="491" spans="1:7">
@@ -13329,7 +13329,7 @@
         <v>588</v>
       </c>
       <c r="G491">
-        <v>6.070153065964875</v>
+        <v>6.070153065964871</v>
       </c>
     </row>
     <row r="492" spans="1:7">
@@ -13352,7 +13352,7 @@
         <v>588</v>
       </c>
       <c r="G492">
-        <v>6.072798071663894</v>
+        <v>6.072798071663891</v>
       </c>
     </row>
     <row r="493" spans="1:7">
@@ -13375,7 +13375,7 @@
         <v>586</v>
       </c>
       <c r="G493">
-        <v>6.072798071663894</v>
+        <v>6.072798071663891</v>
       </c>
     </row>
     <row r="494" spans="1:7">
@@ -13398,7 +13398,7 @@
         <v>588</v>
       </c>
       <c r="G494">
-        <v>5.520953286924958</v>
+        <v>5.520953286924954</v>
       </c>
     </row>
     <row r="495" spans="1:7">
@@ -13421,7 +13421,7 @@
         <v>588</v>
       </c>
       <c r="G495">
-        <v>6.079415866335204</v>
+        <v>6.079415866335201</v>
       </c>
     </row>
     <row r="496" spans="1:7">
@@ -13444,7 +13444,7 @@
         <v>588</v>
       </c>
       <c r="G496">
-        <v>6.072798071663894</v>
+        <v>6.072798071663891</v>
       </c>
     </row>
     <row r="497" spans="1:7">
@@ -13467,7 +13467,7 @@
         <v>592</v>
       </c>
       <c r="G497">
-        <v>6.072798071663894</v>
+        <v>6.072798071663891</v>
       </c>
     </row>
     <row r="498" spans="1:7">
@@ -13490,7 +13490,7 @@
         <v>588</v>
       </c>
       <c r="G498">
-        <v>6.072798071663894</v>
+        <v>6.072798071663891</v>
       </c>
     </row>
     <row r="499" spans="1:7">
@@ -13513,7 +13513,7 @@
         <v>588</v>
       </c>
       <c r="G499">
-        <v>6.059820639635048</v>
+        <v>6.059820639635046</v>
       </c>
     </row>
     <row r="500" spans="1:7">
@@ -13536,7 +13536,7 @@
         <v>588</v>
       </c>
       <c r="G500">
-        <v>6.152174656094856</v>
+        <v>6.152174656094854</v>
       </c>
     </row>
     <row r="501" spans="1:7">
@@ -13556,7 +13556,7 @@
         <v>603</v>
       </c>
       <c r="G501">
-        <v>5.675611165067084</v>
+        <v>5.675611165067086</v>
       </c>
     </row>
     <row r="502" spans="1:7">
@@ -13602,7 +13602,7 @@
         <v>603</v>
       </c>
       <c r="G503">
-        <v>5.79792846811729</v>
+        <v>5.797928468117292</v>
       </c>
     </row>
     <row r="504" spans="1:7">
@@ -13625,7 +13625,7 @@
         <v>603</v>
       </c>
       <c r="G504">
-        <v>6.236297757682336</v>
+        <v>6.236297757682338</v>
       </c>
     </row>
     <row r="505" spans="1:7">
@@ -13648,7 +13648,7 @@
         <v>603</v>
       </c>
       <c r="G505">
-        <v>5.864112222453321</v>
+        <v>5.864112222453323</v>
       </c>
     </row>
     <row r="506" spans="1:7">
@@ -13694,7 +13694,7 @@
         <v>603</v>
       </c>
       <c r="G507">
-        <v>5.448603901836626</v>
+        <v>5.448603901836624</v>
       </c>
     </row>
     <row r="508" spans="1:7">
@@ -13717,7 +13717,7 @@
         <v>603</v>
       </c>
       <c r="G508">
-        <v>5.848354247680304</v>
+        <v>5.848354247680306</v>
       </c>
     </row>
     <row r="509" spans="1:7">
@@ -13740,7 +13740,7 @@
         <v>603</v>
       </c>
       <c r="G509">
-        <v>5.885848920166075</v>
+        <v>5.885848920166077</v>
       </c>
     </row>
     <row r="510" spans="1:7">
@@ -13878,7 +13878,7 @@
         <v>603</v>
       </c>
       <c r="G515">
-        <v>5.672841167224386</v>
+        <v>5.672841167224388</v>
       </c>
     </row>
     <row r="516" spans="1:7">
@@ -13901,7 +13901,7 @@
         <v>603</v>
       </c>
       <c r="G516">
-        <v>5.883836543855721</v>
+        <v>5.883836543855723</v>
       </c>
     </row>
     <row r="517" spans="1:7">
@@ -13924,7 +13924,7 @@
         <v>603</v>
       </c>
       <c r="G517">
-        <v>5.467815024372203</v>
+        <v>5.467815024372205</v>
       </c>
     </row>
     <row r="518" spans="1:7">
@@ -13947,7 +13947,7 @@
         <v>603</v>
       </c>
       <c r="G518">
-        <v>5.836314700964658</v>
+        <v>5.836314700964659</v>
       </c>
     </row>
     <row r="519" spans="1:7">
@@ -13993,7 +13993,7 @@
         <v>603</v>
       </c>
       <c r="G520">
-        <v>5.783665669904408</v>
+        <v>5.783665669904409</v>
       </c>
     </row>
     <row r="521" spans="1:7">
@@ -14016,7 +14016,7 @@
         <v>603</v>
       </c>
       <c r="G521">
-        <v>5.580487150764578</v>
+        <v>5.58048715076458</v>
       </c>
     </row>
     <row r="522" spans="1:7">
@@ -14062,7 +14062,7 @@
         <v>603</v>
       </c>
       <c r="G523">
-        <v>5.827224965469058</v>
+        <v>5.82722496546906</v>
       </c>
     </row>
     <row r="524" spans="1:7">
@@ -14085,7 +14085,7 @@
         <v>603</v>
       </c>
       <c r="G524">
-        <v>6.033131665641048</v>
+        <v>6.03313166564105</v>
       </c>
     </row>
     <row r="525" spans="1:7">
@@ -14108,7 +14108,7 @@
         <v>603</v>
       </c>
       <c r="G525">
-        <v>5.504942948531691</v>
+        <v>5.504942948531693</v>
       </c>
     </row>
     <row r="526" spans="1:7">
@@ -14131,7 +14131,7 @@
         <v>603</v>
       </c>
       <c r="G526">
-        <v>5.398549644140576</v>
+        <v>5.398549644140577</v>
       </c>
     </row>
     <row r="527" spans="1:7">
@@ -14154,7 +14154,7 @@
         <v>595</v>
       </c>
       <c r="G527">
-        <v>6.200063964574254</v>
+        <v>6.200063964574253</v>
       </c>
     </row>
     <row r="528" spans="1:7">
@@ -14177,7 +14177,7 @@
         <v>595</v>
       </c>
       <c r="G528">
-        <v>5.990420200167018</v>
+        <v>5.990420200167015</v>
       </c>
     </row>
     <row r="529" spans="1:7">
@@ -14200,7 +14200,7 @@
         <v>595</v>
       </c>
       <c r="G529">
-        <v>6.215224048258537</v>
+        <v>6.215224048258535</v>
       </c>
     </row>
     <row r="530" spans="1:7">
@@ -14223,7 +14223,7 @@
         <v>595</v>
       </c>
       <c r="G530">
-        <v>6.132495574029623</v>
+        <v>6.132495574029622</v>
       </c>
     </row>
     <row r="531" spans="1:7">
@@ -14269,7 +14269,7 @@
         <v>595</v>
       </c>
       <c r="G532">
-        <v>6.23988265346062</v>
+        <v>6.239882653460616</v>
       </c>
     </row>
     <row r="533" spans="1:7">
@@ -14292,7 +14292,7 @@
         <v>595</v>
       </c>
       <c r="G533">
-        <v>6.254598389581708</v>
+        <v>6.254598389581706</v>
       </c>
     </row>
     <row r="534" spans="1:7">
@@ -14315,7 +14315,7 @@
         <v>595</v>
       </c>
       <c r="G534">
-        <v>6.381620557297773</v>
+        <v>6.381620557297771</v>
       </c>
     </row>
     <row r="535" spans="1:7">
@@ -14338,7 +14338,7 @@
         <v>595</v>
       </c>
       <c r="G535">
-        <v>5.903769218104485</v>
+        <v>5.903769218104482</v>
       </c>
     </row>
     <row r="536" spans="1:7">
@@ -14361,7 +14361,7 @@
         <v>595</v>
       </c>
       <c r="G536">
-        <v>6.166989644743333</v>
+        <v>6.166989644743331</v>
       </c>
     </row>
     <row r="537" spans="1:7">
@@ -14384,7 +14384,7 @@
         <v>595</v>
       </c>
       <c r="G537">
-        <v>6.398064183235562</v>
+        <v>6.398064183235561</v>
       </c>
     </row>
     <row r="538" spans="1:7">
@@ -14407,7 +14407,7 @@
         <v>595</v>
       </c>
       <c r="G538">
-        <v>6.169634650442352</v>
+        <v>6.16963465044235</v>
       </c>
     </row>
     <row r="539" spans="1:7">
@@ -14430,7 +14430,7 @@
         <v>595</v>
       </c>
       <c r="G539">
-        <v>6.013066636278928</v>
+        <v>6.013066636278926</v>
       </c>
     </row>
     <row r="540" spans="1:7">
@@ -14453,7 +14453,7 @@
         <v>595</v>
       </c>
       <c r="G540">
-        <v>6.08961230842653</v>
+        <v>6.089612308426529</v>
       </c>
     </row>
     <row r="541" spans="1:7">
@@ -14476,7 +14476,7 @@
         <v>595</v>
       </c>
       <c r="G541">
-        <v>6.338887063091369</v>
+        <v>6.338887063091366</v>
       </c>
     </row>
     <row r="542" spans="1:7">
@@ -14499,7 +14499,7 @@
         <v>595</v>
       </c>
       <c r="G542">
-        <v>6.104220609741033</v>
+        <v>6.10422060974103</v>
       </c>
     </row>
     <row r="543" spans="1:7">
@@ -14522,7 +14522,7 @@
         <v>595</v>
       </c>
       <c r="G543">
-        <v>6.104220609741033</v>
+        <v>6.10422060974103</v>
       </c>
     </row>
     <row r="544" spans="1:7">
@@ -14545,7 +14545,7 @@
         <v>595</v>
       </c>
       <c r="G544">
-        <v>6.156657218413506</v>
+        <v>6.156657218413504</v>
       </c>
     </row>
     <row r="545" spans="1:7">
@@ -14568,7 +14568,7 @@
         <v>595</v>
       </c>
       <c r="G545">
-        <v>6.120707972282513</v>
+        <v>6.120707972282511</v>
       </c>
     </row>
     <row r="546" spans="1:7">
@@ -14591,7 +14591,7 @@
         <v>595</v>
       </c>
       <c r="G546">
-        <v>6.11127173400202</v>
+        <v>6.111271734002016</v>
       </c>
     </row>
     <row r="547" spans="1:7">
@@ -14614,7 +14614,7 @@
         <v>595</v>
       </c>
       <c r="G547">
-        <v>6.138002771124516</v>
+        <v>6.138002771124515</v>
       </c>
     </row>
     <row r="548" spans="1:7">
@@ -14637,7 +14637,7 @@
         <v>595</v>
       </c>
       <c r="G548">
-        <v>6.156657218413506</v>
+        <v>6.156657218413504</v>
       </c>
     </row>
     <row r="549" spans="1:7">
@@ -14660,7 +14660,7 @@
         <v>595</v>
       </c>
       <c r="G549">
-        <v>6.20936095093909</v>
+        <v>6.209360950939089</v>
       </c>
     </row>
     <row r="550" spans="1:7">
@@ -14683,7 +14683,7 @@
         <v>595</v>
       </c>
       <c r="G550">
-        <v>6.153887220570808</v>
+        <v>6.153887220570804</v>
       </c>
     </row>
     <row r="551" spans="1:7">
@@ -14706,7 +14706,7 @@
         <v>595</v>
       </c>
       <c r="G551">
-        <v>6.280459153122373</v>
+        <v>6.280459153122371</v>
       </c>
     </row>
     <row r="552" spans="1:7">
@@ -14729,7 +14729,7 @@
         <v>584</v>
       </c>
       <c r="G552">
-        <v>5.762548912369678</v>
+        <v>5.762548912369676</v>
       </c>
     </row>
     <row r="553" spans="1:7">
@@ -14752,7 +14752,7 @@
         <v>586</v>
       </c>
       <c r="G553">
-        <v>6.095224854349369</v>
+        <v>6.095224854349365</v>
       </c>
     </row>
     <row r="554" spans="1:7">
@@ -14775,7 +14775,7 @@
         <v>587</v>
       </c>
       <c r="G554">
-        <v>6.20691835388618</v>
+        <v>6.206918353886182</v>
       </c>
     </row>
     <row r="555" spans="1:7">
@@ -14798,7 +14798,7 @@
         <v>601</v>
       </c>
       <c r="G555">
-        <v>5.81087881388654</v>
+        <v>5.810878813886538</v>
       </c>
     </row>
     <row r="556" spans="1:7">
@@ -14821,7 +14821,7 @@
         <v>596</v>
       </c>
       <c r="G556">
-        <v>6.011279728293377</v>
+        <v>6.011279728293379</v>
       </c>
     </row>
     <row r="557" spans="1:7">
@@ -14844,7 +14844,7 @@
         <v>601</v>
       </c>
       <c r="G557">
-        <v>6.387232418172636</v>
+        <v>6.387232418172638</v>
       </c>
     </row>
     <row r="558" spans="1:7">
@@ -14867,7 +14867,7 @@
         <v>599</v>
       </c>
       <c r="G558">
-        <v>6.247087670835549</v>
+        <v>6.24708767083555</v>
       </c>
     </row>
     <row r="559" spans="1:7">
@@ -14890,7 +14890,7 @@
         <v>584</v>
       </c>
       <c r="G559">
-        <v>5.889729567388049</v>
+        <v>5.889729567388048</v>
       </c>
     </row>
     <row r="560" spans="1:7">
@@ -14913,7 +14913,7 @@
         <v>587</v>
       </c>
       <c r="G560">
-        <v>6.18283264566051</v>
+        <v>6.182832645660514</v>
       </c>
     </row>
     <row r="561" spans="1:7">
@@ -14979,7 +14979,7 @@
         <v>592</v>
       </c>
       <c r="G563">
-        <v>5.382083788692126</v>
+        <v>5.382083788692124</v>
       </c>
     </row>
     <row r="564" spans="1:7">
@@ -14999,7 +14999,7 @@
         <v>593</v>
       </c>
       <c r="G564">
-        <v>6.047458989540634</v>
+        <v>6.047458989540636</v>
       </c>
     </row>
     <row r="565" spans="1:7">
@@ -15019,7 +15019,7 @@
         <v>596</v>
       </c>
       <c r="G565">
-        <v>5.929600270983289</v>
+        <v>5.929600270983291</v>
       </c>
     </row>
     <row r="566" spans="1:7">
@@ -15065,7 +15065,7 @@
         <v>584</v>
       </c>
       <c r="G567">
-        <v>5.953996954614383</v>
+        <v>5.953996954614381</v>
       </c>
     </row>
     <row r="568" spans="1:7">
@@ -15111,7 +15111,7 @@
         <v>587</v>
       </c>
       <c r="G569">
-        <v>5.64523468927344</v>
+        <v>5.645234689273441</v>
       </c>
     </row>
     <row r="570" spans="1:7">
@@ -15134,7 +15134,7 @@
         <v>589</v>
       </c>
       <c r="G570">
-        <v>5.928094681745857</v>
+        <v>5.928094681745859</v>
       </c>
     </row>
     <row r="571" spans="1:7">
@@ -15157,7 +15157,7 @@
         <v>591</v>
       </c>
       <c r="G571">
-        <v>5.832181069408642</v>
+        <v>5.832181069408644</v>
       </c>
     </row>
     <row r="572" spans="1:7">
@@ -15180,7 +15180,7 @@
         <v>591</v>
       </c>
       <c r="G572">
-        <v>6.024982972882083</v>
+        <v>6.024982972882085</v>
       </c>
     </row>
     <row r="573" spans="1:7">
@@ -15203,7 +15203,7 @@
         <v>593</v>
       </c>
       <c r="G573">
-        <v>6.007273637240776</v>
+        <v>6.007273637240778</v>
       </c>
     </row>
     <row r="574" spans="1:7">
@@ -15249,7 +15249,7 @@
         <v>598</v>
       </c>
       <c r="G575">
-        <v>5.273235109311828</v>
+        <v>5.273235109311826</v>
       </c>
     </row>
     <row r="576" spans="1:7">
@@ -15292,7 +15292,7 @@
         <v>599</v>
       </c>
       <c r="G577">
-        <v>5.897754440287982</v>
+        <v>5.897754440287984</v>
       </c>
     </row>
     <row r="578" spans="1:7">
@@ -15315,7 +15315,7 @@
         <v>600</v>
       </c>
       <c r="G578">
-        <v>6.424824511127203</v>
+        <v>6.424824511127205</v>
       </c>
     </row>
     <row r="579" spans="1:7">
@@ -15355,7 +15355,7 @@
         <v>601</v>
       </c>
       <c r="G580">
-        <v>5.812180675076113</v>
+        <v>5.812180675076109</v>
       </c>
     </row>
     <row r="581" spans="1:7">
@@ -15401,7 +15401,7 @@
         <v>588</v>
       </c>
       <c r="G582">
-        <v>5.782759118708539</v>
+        <v>5.782759118708538</v>
       </c>
     </row>
     <row r="583" spans="1:7">
@@ -15421,7 +15421,7 @@
         <v>588</v>
       </c>
       <c r="G583">
-        <v>5.853326360259067</v>
+        <v>5.853326360259063</v>
       </c>
     </row>
     <row r="584" spans="1:7">
@@ -15444,7 +15444,7 @@
         <v>588</v>
       </c>
       <c r="G584">
-        <v>5.968482875319716</v>
+        <v>5.968482875319713</v>
       </c>
     </row>
     <row r="585" spans="1:7">
@@ -15490,7 +15490,7 @@
         <v>587</v>
       </c>
       <c r="G586">
-        <v>5.899038171195639</v>
+        <v>5.899038171195641</v>
       </c>
     </row>
     <row r="587" spans="1:7">
@@ -15513,7 +15513,7 @@
         <v>594</v>
       </c>
       <c r="G587">
-        <v>5.417012854063221</v>
+        <v>5.417012854063217</v>
       </c>
     </row>
     <row r="588" spans="1:7">
@@ -15536,7 +15536,7 @@
         <v>602</v>
       </c>
       <c r="G588">
-        <v>6.042910399477532</v>
+        <v>6.042910399477534</v>
       </c>
     </row>
     <row r="589" spans="1:7">
@@ -15582,7 +15582,7 @@
         <v>585</v>
       </c>
       <c r="G590">
-        <v>5.505040788127086</v>
+        <v>5.505040788127082</v>
       </c>
     </row>
     <row r="591" spans="1:7">
@@ -15605,7 +15605,7 @@
         <v>594</v>
       </c>
       <c r="G591">
-        <v>6.153391565131598</v>
+        <v>6.153391565131595</v>
       </c>
     </row>
     <row r="592" spans="1:7">
@@ -15628,7 +15628,7 @@
         <v>599</v>
       </c>
       <c r="G592">
-        <v>5.493977831168082</v>
+        <v>5.493977831168084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>